<commit_message>
🤖 Publica dados no site (05/11/2025 10:49)
</commit_message>
<xml_diff>
--- a/site/downloads/UNICAMP _ Acesso Direto.xlsx
+++ b/site/downloads/UNICAMP _ Acesso Direto.xlsx
@@ -815,7 +815,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>386</t>
+          <t>387</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>27,57</t>
+          <t>27,64</t>
         </is>
       </c>
     </row>

</xml_diff>